<commit_message>
feat(excel):fix the ReadFromSheet function
</commit_message>
<xml_diff>
--- a/基础信息.xlsx
+++ b/基础信息.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20752" windowHeight="9555" tabRatio="633"/>
+    <workbookView windowWidth="27600" windowHeight="13160" tabRatio="633"/>
   </bookViews>
   <sheets>
     <sheet name="江苏城市分级" sheetId="2" r:id="rId1"/>
@@ -12,25 +12,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">江苏城市分级!$A$1:$K$14</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="80">
   <si>
     <t>序号</t>
   </si>
@@ -60,6 +47,9 @@
   </si>
   <si>
     <t>厂家</t>
+  </si>
+  <si>
+    <t>序号2</t>
   </si>
   <si>
     <t>城市分类</t>
@@ -953,13 +943,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1294,23 +1284,23 @@
   <dimension ref="A1:M34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="11.6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.6"/>
   <cols>
-    <col min="1" max="1" width="4.44247787610619" style="1" customWidth="1"/>
-    <col min="2" max="2" width="7.11504424778761" style="2" customWidth="1"/>
+    <col min="1" max="1" width="4.44117647058824" style="1" customWidth="1"/>
+    <col min="2" max="2" width="7.11764705882353" style="2" customWidth="1"/>
     <col min="3" max="3" width="6" style="3" customWidth="1"/>
-    <col min="4" max="4" width="4.44247787610619" style="3" customWidth="1"/>
+    <col min="4" max="4" width="4.44117647058824" style="3" customWidth="1"/>
     <col min="5" max="5" width="9" style="3"/>
-    <col min="6" max="6" width="7.44247787610619" style="4" customWidth="1"/>
+    <col min="6" max="6" width="7.44117647058824" style="4" customWidth="1"/>
     <col min="7" max="7" width="6" style="3" customWidth="1"/>
     <col min="8" max="8" width="9" style="2"/>
-    <col min="9" max="9" width="13.3362831858407" style="2" customWidth="1"/>
-    <col min="10" max="10" width="10.4424778761062" style="1" customWidth="1"/>
+    <col min="9" max="9" width="13.3382352941176" style="2" customWidth="1"/>
+    <col min="10" max="10" width="10.4411764705882" style="1" customWidth="1"/>
     <col min="11" max="11" width="9" style="2"/>
-    <col min="12" max="12" width="14.4424778761062" style="2" customWidth="1"/>
+    <col min="12" max="12" width="14.4411764705882" style="2" customWidth="1"/>
     <col min="13" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
@@ -1330,7 +1320,7 @@
       <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="10" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="7" t="s">
@@ -1346,542 +1336,542 @@
         <v>9</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L1" s="13" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M1" s="13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" ht="11.65" spans="1:13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" ht="14" spans="1:13">
       <c r="A2" s="5">
         <f>SUBTOTAL(103,B$2:B2)*1</f>
         <v>1</v>
       </c>
-      <c r="B2" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="10" t="s">
+      <c r="B2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="C2" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="10">
+      <c r="D2" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="9">
         <v>210000</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="10" t="s">
         <v>16</v>
       </c>
+      <c r="G2" s="9" t="s">
+        <v>17</v>
+      </c>
       <c r="H2" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K2" s="5">
         <v>1</v>
       </c>
       <c r="L2" s="13" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M2" s="13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" ht="11.65" spans="1:13">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" ht="14" spans="1:13">
       <c r="A3" s="5">
         <f>SUBTOTAL(103,B$2:B3)*1</f>
         <v>2</v>
       </c>
-      <c r="B3" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="10" t="s">
+      <c r="B3" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="10">
+      <c r="D3" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="9">
         <v>215000</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" s="10" t="s">
         <v>24</v>
       </c>
+      <c r="G3" s="9" t="s">
+        <v>25</v>
+      </c>
       <c r="H3" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K3" s="5">
         <v>2</v>
       </c>
       <c r="L3" s="13" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M3" s="13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" ht="11.65" spans="1:13">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" ht="14" spans="1:13">
       <c r="A4" s="5">
         <f>SUBTOTAL(103,B$2:B4)*1</f>
         <v>3</v>
       </c>
-      <c r="B4" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="10" t="s">
+      <c r="B4" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="10">
+      <c r="D4" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="9">
         <v>214000</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="G4" s="10" t="s">
         <v>28</v>
       </c>
+      <c r="G4" s="9" t="s">
+        <v>29</v>
+      </c>
       <c r="H4" s="12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K4" s="5">
         <v>3</v>
       </c>
       <c r="L4" s="13" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M4" s="13" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" ht="11.65" spans="1:13">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" ht="14" spans="1:13">
       <c r="A5" s="5">
         <f>SUBTOTAL(103,B$2:B5)*1</f>
         <v>4</v>
       </c>
-      <c r="B5" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="D5" s="10" t="s">
+      <c r="B5" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="E5" s="10">
+      <c r="D5" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="9">
         <v>213000</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="G5" s="10" t="s">
         <v>35</v>
       </c>
+      <c r="G5" s="9" t="s">
+        <v>36</v>
+      </c>
       <c r="H5" s="12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="K5" s="5">
         <v>4</v>
       </c>
       <c r="L5" s="13" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="M5" s="13" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" ht="11.65" spans="1:13">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" ht="14" spans="1:13">
       <c r="A6" s="5">
         <f>SUBTOTAL(103,B$2:B6)*1</f>
         <v>5</v>
       </c>
-      <c r="B6" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="D6" s="10" t="s">
+      <c r="B6" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="E6" s="10">
+      <c r="D6" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" s="9">
         <v>212000</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="G6" s="10" t="s">
         <v>41</v>
       </c>
+      <c r="G6" s="9" t="s">
+        <v>42</v>
+      </c>
       <c r="H6" s="12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I6" s="12" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K6" s="5">
         <v>5</v>
       </c>
       <c r="L6" s="13" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="M6" s="13" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" ht="11.65" spans="1:13">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" ht="14" spans="1:13">
       <c r="A7" s="5">
         <f>SUBTOTAL(103,B$2:B7)*1</f>
         <v>6</v>
       </c>
-      <c r="B7" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="D7" s="10" t="s">
+      <c r="B7" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="E7" s="10">
+      <c r="D7" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" s="9">
         <v>225000</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="G7" s="10" t="s">
         <v>45</v>
       </c>
+      <c r="G7" s="9" t="s">
+        <v>46</v>
+      </c>
       <c r="H7" s="12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I7" s="12" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K7" s="5">
         <v>6</v>
       </c>
       <c r="L7" s="13" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="M7" s="13" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" ht="11.65" spans="1:13">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" ht="14" spans="1:13">
       <c r="A8" s="5">
         <f>SUBTOTAL(103,B$2:B8)*1</f>
         <v>7</v>
       </c>
-      <c r="B8" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="D8" s="10" t="s">
+      <c r="B8" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="E8" s="10">
+      <c r="D8" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" s="9">
         <v>225300</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="G8" s="10" t="s">
         <v>50</v>
       </c>
+      <c r="G8" s="9" t="s">
+        <v>51</v>
+      </c>
       <c r="H8" s="12" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I8" s="12" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="K8" s="5">
         <v>7</v>
       </c>
       <c r="L8" s="13"/>
       <c r="M8" s="13" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" ht="11.65" spans="1:13">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" ht="14" spans="1:13">
       <c r="A9" s="5">
         <f>SUBTOTAL(103,B$2:B9)*1</f>
         <v>8</v>
       </c>
-      <c r="B9" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="D9" s="10" t="s">
+      <c r="B9" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="E9" s="10">
+      <c r="D9" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9" s="9">
         <v>226000</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="G9" s="10" t="s">
         <v>57</v>
       </c>
+      <c r="G9" s="9" t="s">
+        <v>58</v>
+      </c>
       <c r="H9" s="12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="K9" s="5">
         <v>8</v>
       </c>
       <c r="L9" s="13" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="M9" s="13" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" ht="11.65" spans="1:13">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" ht="14" spans="1:13">
       <c r="A10" s="5">
         <f>SUBTOTAL(103,B$2:B10)*1</f>
         <v>9</v>
       </c>
-      <c r="B10" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="D10" s="10" t="s">
+      <c r="B10" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="E10" s="10">
+      <c r="D10" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="E10" s="9">
         <v>224000</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="G10" s="10" t="s">
         <v>62</v>
       </c>
+      <c r="G10" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="H10" s="12" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="K10" s="5">
         <v>9</v>
       </c>
       <c r="L10" s="13"/>
       <c r="M10" s="13" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" ht="11.65" spans="1:13">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" ht="14" spans="1:13">
       <c r="A11" s="5">
         <f>SUBTOTAL(103,B$2:B11)*1</f>
         <v>10</v>
       </c>
-      <c r="B11" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="D11" s="10" t="s">
+      <c r="B11" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="E11" s="10">
+      <c r="D11" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="E11" s="9">
         <v>223001</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="G11" s="10" t="s">
         <v>66</v>
       </c>
+      <c r="G11" s="9" t="s">
+        <v>67</v>
+      </c>
       <c r="H11" s="12" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I11" s="12" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K11" s="5">
         <v>10</v>
       </c>
       <c r="L11" s="13"/>
       <c r="M11" s="13" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" ht="11.65" spans="1:13">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" ht="14" spans="1:13">
       <c r="A12" s="5">
         <f>SUBTOTAL(103,B$2:B12)*1</f>
         <v>11</v>
       </c>
-      <c r="B12" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="D12" s="10" t="s">
+      <c r="B12" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="E12" s="10">
+      <c r="D12" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="E12" s="9">
         <v>223800</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="G12" s="10" t="s">
         <v>70</v>
       </c>
+      <c r="G12" s="9" t="s">
+        <v>71</v>
+      </c>
       <c r="H12" s="12" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I12" s="12" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K12" s="5">
         <v>11</v>
       </c>
       <c r="L12" s="13"/>
       <c r="M12" s="13" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" ht="11.65" spans="1:13">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" ht="14" spans="1:13">
       <c r="A13" s="5">
         <f>SUBTOTAL(103,B$2:B13)*1</f>
         <v>12</v>
       </c>
-      <c r="B13" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="D13" s="10" t="s">
+      <c r="B13" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="E13" s="10">
+      <c r="D13" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="E13" s="9">
         <v>221000</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="G13" s="10" t="s">
-        <v>51</v>
+        <v>74</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>52</v>
       </c>
       <c r="H13" s="12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I13" s="12" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K13" s="5">
         <v>12</v>
       </c>
       <c r="L13" s="13" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="M13" s="13" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" ht="11.65" spans="1:13">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" ht="14" spans="1:13">
       <c r="A14" s="5">
         <f>SUBTOTAL(103,B$2:B14)*1</f>
         <v>13</v>
       </c>
-      <c r="B14" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="D14" s="10" t="s">
+      <c r="B14" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="E14" s="10">
+      <c r="D14" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="E14" s="9">
         <v>222000</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="G14" s="10" t="s">
         <v>78</v>
       </c>
+      <c r="G14" s="9" t="s">
+        <v>79</v>
+      </c>
       <c r="H14" s="12" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I14" s="12" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="K14" s="5">
         <v>13</v>

</xml_diff>

<commit_message>
feat(excel): Update Read function
</commit_message>
<xml_diff>
--- a/基础信息.xlsx
+++ b/基础信息.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27600" windowHeight="13160" tabRatio="633"/>
+    <workbookView windowWidth="27952" windowHeight="12255" tabRatio="633"/>
   </bookViews>
   <sheets>
     <sheet name="江苏城市分级" sheetId="2" r:id="rId1"/>
@@ -12,12 +12,25 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">江苏城市分级!$A$1:$K$14</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="82">
   <si>
     <t>序号</t>
   </si>
@@ -56,6 +69,12 @@
   </si>
   <si>
     <t>城市分类2</t>
+  </si>
+  <si>
+    <t>是的</t>
+  </si>
+  <si>
+    <t>日期</t>
   </si>
   <si>
     <t>江苏</t>
@@ -263,11 +282,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="yyyy/m/d;@"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -918,7 +938,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -943,15 +963,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -959,6 +979,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1281,30 +1304,32 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:M34"/>
+  <dimension ref="A1:O34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="11.6"/>
   <cols>
-    <col min="1" max="1" width="4.44117647058824" style="1" customWidth="1"/>
-    <col min="2" max="2" width="7.11764705882353" style="2" customWidth="1"/>
+    <col min="1" max="1" width="4.44247787610619" style="1" customWidth="1"/>
+    <col min="2" max="2" width="7.11504424778761" style="2" customWidth="1"/>
     <col min="3" max="3" width="6" style="3" customWidth="1"/>
-    <col min="4" max="4" width="4.44117647058824" style="3" customWidth="1"/>
+    <col min="4" max="4" width="4.44247787610619" style="3" customWidth="1"/>
     <col min="5" max="5" width="9" style="3"/>
-    <col min="6" max="6" width="7.44117647058824" style="4" customWidth="1"/>
+    <col min="6" max="6" width="7.44247787610619" style="4" customWidth="1"/>
     <col min="7" max="7" width="6" style="3" customWidth="1"/>
     <col min="8" max="8" width="9" style="2"/>
-    <col min="9" max="9" width="13.3382352941176" style="2" customWidth="1"/>
-    <col min="10" max="10" width="10.4411764705882" style="1" customWidth="1"/>
+    <col min="9" max="9" width="13.3362831858407" style="2" customWidth="1"/>
+    <col min="10" max="10" width="10.4424778761062" style="1" customWidth="1"/>
     <col min="11" max="11" width="9" style="2"/>
-    <col min="12" max="12" width="14.4411764705882" style="2" customWidth="1"/>
-    <col min="13" max="16384" width="9" style="2"/>
+    <col min="12" max="12" width="14.4424778761062" style="2" customWidth="1"/>
+    <col min="13" max="14" width="9" style="2"/>
+    <col min="15" max="15" width="12.646017699115" style="2"/>
+    <col min="16" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" ht="20.25" customHeight="1" spans="1:13">
+    <row r="1" ht="20.25" customHeight="1" spans="1:15">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1320,7 +1345,7 @@
       <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="8" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="7" t="s">
@@ -1344,540 +1369,624 @@
       <c r="M1" s="13" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" ht="14" spans="1:13">
+      <c r="N1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" ht="11.65" spans="1:15">
       <c r="A2" s="5">
         <f>SUBTOTAL(103,B$2:B2)*1</f>
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="9" t="s">
+      <c r="B2" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="9">
+      <c r="C2" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="10">
         <v>210000</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>19</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="K2" s="5">
         <v>1</v>
       </c>
       <c r="L2" s="13" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="M2" s="13" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" ht="14" spans="1:13">
+        <v>23</v>
+      </c>
+      <c r="N2" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="O2" s="14">
+        <v>45300</v>
+      </c>
+    </row>
+    <row r="3" ht="11.65" spans="1:15">
       <c r="A3" s="5">
         <f>SUBTOTAL(103,B$2:B3)*1</f>
         <v>2</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" s="9">
+      <c r="B3" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="10">
         <v>215000</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>27</v>
       </c>
       <c r="H3" s="12" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="K3" s="5">
         <v>2</v>
       </c>
       <c r="L3" s="13" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="M3" s="13" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" ht="14" spans="1:13">
+        <v>23</v>
+      </c>
+      <c r="N3" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="O3" s="14">
+        <v>45301</v>
+      </c>
+    </row>
+    <row r="4" ht="11.65" spans="1:15">
       <c r="A4" s="5">
         <f>SUBTOTAL(103,B$2:B4)*1</f>
         <v>3</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" s="9">
+      <c r="B4" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="10">
         <v>214000</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>31</v>
       </c>
       <c r="H4" s="12" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="K4" s="5">
         <v>3</v>
       </c>
       <c r="L4" s="13" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="M4" s="13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" ht="14" spans="1:13">
+        <v>34</v>
+      </c>
+      <c r="N4" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="O4" s="14">
+        <v>45302</v>
+      </c>
+    </row>
+    <row r="5" ht="11.65" spans="1:15">
       <c r="A5" s="5">
         <f>SUBTOTAL(103,B$2:B5)*1</f>
         <v>4</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="E5" s="9">
+      <c r="B5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" s="10">
         <v>213000</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>36</v>
+        <v>37</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>38</v>
       </c>
       <c r="H5" s="12" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="K5" s="5">
         <v>4</v>
       </c>
       <c r="L5" s="13" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="M5" s="13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" ht="14" spans="1:13">
+        <v>34</v>
+      </c>
+      <c r="N5" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="O5" s="14">
+        <v>45303</v>
+      </c>
+    </row>
+    <row r="6" ht="11.65" spans="1:15">
       <c r="A6" s="5">
         <f>SUBTOTAL(103,B$2:B6)*1</f>
         <v>5</v>
       </c>
-      <c r="B6" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="E6" s="9">
+      <c r="B6" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" s="10">
         <v>212000</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>42</v>
+        <v>43</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>44</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="I6" s="12" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="K6" s="5">
         <v>5</v>
       </c>
       <c r="L6" s="13" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="M6" s="13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" ht="14" spans="1:13">
+        <v>34</v>
+      </c>
+      <c r="N6" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="O6" s="14">
+        <v>45304</v>
+      </c>
+    </row>
+    <row r="7" ht="11.65" spans="1:15">
       <c r="A7" s="5">
         <f>SUBTOTAL(103,B$2:B7)*1</f>
         <v>6</v>
       </c>
-      <c r="B7" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="E7" s="9">
+      <c r="B7" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" s="10">
         <v>225000</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>46</v>
+        <v>47</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>48</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="I7" s="12" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="K7" s="5">
         <v>6</v>
       </c>
       <c r="L7" s="13" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="M7" s="13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" ht="14" spans="1:13">
+        <v>34</v>
+      </c>
+      <c r="N7" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="O7" s="14">
+        <v>45305</v>
+      </c>
+    </row>
+    <row r="8" ht="11.65" spans="1:15">
       <c r="A8" s="5">
         <f>SUBTOTAL(103,B$2:B8)*1</f>
         <v>7</v>
       </c>
-      <c r="B8" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="E8" s="9">
+      <c r="B8" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" s="10">
         <v>225300</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>51</v>
+        <v>52</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>53</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="I8" s="12" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="K8" s="5">
         <v>7</v>
       </c>
       <c r="L8" s="13"/>
       <c r="M8" s="13" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" ht="14" spans="1:13">
+        <v>32</v>
+      </c>
+      <c r="N8" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="O8" s="14">
+        <v>45306</v>
+      </c>
+    </row>
+    <row r="9" ht="11.65" spans="1:15">
       <c r="A9" s="5">
         <f>SUBTOTAL(103,B$2:B9)*1</f>
         <v>8</v>
       </c>
-      <c r="B9" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="E9" s="9">
+      <c r="B9" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" s="10">
         <v>226000</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>60</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="K9" s="5">
         <v>8</v>
       </c>
       <c r="L9" s="13" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="M9" s="13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" ht="14" spans="1:13">
+        <v>34</v>
+      </c>
+      <c r="N9" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="O9" s="14">
+        <v>45307</v>
+      </c>
+    </row>
+    <row r="10" ht="11.65" spans="1:15">
       <c r="A10" s="5">
         <f>SUBTOTAL(103,B$2:B10)*1</f>
         <v>9</v>
       </c>
-      <c r="B10" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="E10" s="9">
+      <c r="B10" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="E10" s="10">
         <v>224000</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="G10" s="9" t="s">
-        <v>63</v>
+        <v>64</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>65</v>
       </c>
       <c r="H10" s="12" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="K10" s="5">
         <v>9</v>
       </c>
       <c r="L10" s="13"/>
       <c r="M10" s="13" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" ht="14" spans="1:13">
+        <v>32</v>
+      </c>
+      <c r="N10" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="O10" s="14">
+        <v>45308</v>
+      </c>
+    </row>
+    <row r="11" ht="11.65" spans="1:15">
       <c r="A11" s="5">
         <f>SUBTOTAL(103,B$2:B11)*1</f>
         <v>10</v>
       </c>
-      <c r="B11" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="E11" s="9">
+      <c r="B11" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="E11" s="10">
         <v>223001</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>67</v>
+        <v>68</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>69</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="I11" s="12" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="K11" s="5">
         <v>10</v>
       </c>
       <c r="L11" s="13"/>
       <c r="M11" s="13" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" ht="14" spans="1:13">
+        <v>32</v>
+      </c>
+      <c r="N11" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="O11" s="14">
+        <v>45309</v>
+      </c>
+    </row>
+    <row r="12" ht="11.65" spans="1:15">
       <c r="A12" s="5">
         <f>SUBTOTAL(103,B$2:B12)*1</f>
         <v>11</v>
       </c>
-      <c r="B12" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="E12" s="9">
+      <c r="B12" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="E12" s="10">
         <v>223800</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>71</v>
+        <v>72</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>73</v>
       </c>
       <c r="H12" s="12" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="I12" s="12" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="K12" s="5">
         <v>11</v>
       </c>
       <c r="L12" s="13"/>
       <c r="M12" s="13" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" ht="14" spans="1:13">
+        <v>32</v>
+      </c>
+      <c r="N12" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="O12" s="14">
+        <v>45310</v>
+      </c>
+    </row>
+    <row r="13" ht="11.65" spans="1:15">
       <c r="A13" s="5">
         <f>SUBTOTAL(103,B$2:B13)*1</f>
         <v>12</v>
       </c>
-      <c r="B13" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="E13" s="9">
+      <c r="B13" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="E13" s="10">
         <v>221000</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="G13" s="9" t="s">
-        <v>52</v>
+        <v>76</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>54</v>
       </c>
       <c r="H13" s="12" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="I13" s="12" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="K13" s="5">
         <v>12</v>
       </c>
       <c r="L13" s="13" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="M13" s="13" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" ht="14" spans="1:13">
+        <v>32</v>
+      </c>
+      <c r="N13" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="O13" s="14">
+        <v>45311</v>
+      </c>
+    </row>
+    <row r="14" ht="11.65" spans="1:15">
       <c r="A14" s="5">
         <f>SUBTOTAL(103,B$2:B14)*1</f>
         <v>13</v>
       </c>
-      <c r="B14" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="E14" s="9">
+      <c r="B14" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="E14" s="10">
         <v>222000</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="G14" s="9" t="s">
-        <v>79</v>
+        <v>80</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>81</v>
       </c>
       <c r="H14" s="12" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="I14" s="12" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="K14" s="5">
         <v>13</v>
       </c>
       <c r="L14" s="13"/>
       <c r="M14" s="13"/>
+      <c r="N14" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="O14" s="14">
+        <v>45312</v>
+      </c>
     </row>
     <row r="18" spans="10:10">
       <c r="J18" s="2"/>

</xml_diff>